<commit_message>
new folder for each tournament
</commit_message>
<xml_diff>
--- a/VB2.0_Teams_Sch_Rules_Org/VB2.0__Teams_Rules_Sch_Org.xlsx
+++ b/VB2.0_Teams_Sch_Rules_Org/VB2.0__Teams_Rules_Sch_Org.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24709"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="22880" windowHeight="13140" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="22880" windowHeight="13140" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="4" r:id="rId1"/>
     <sheet name="Teams" sheetId="5" r:id="rId2"/>
-    <sheet name="Rules_old" sheetId="6" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
+    <sheet name="Rules" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="98">
   <si>
     <t>League matches</t>
   </si>
@@ -96,57 +95,6 @@
     <t xml:space="preserve">VolleyBall Tournment 2019  V2.0 </t>
   </si>
   <si>
-    <t>           Winner will get 2 points and the top 4 high scoring teams will play semis. Winner of semis will play finals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           If 2 teams end up having same points, then highest cummulative difference in points will be considered (like NRR)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           Court Switch in the finals can happen only after each set.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rules: 1) Teams will be playing with rotation concept (Players can exchange positions while the ball is in the air during service). </t>
-  </si>
-  <si>
-    <t>Players can swap during the game only side not front and back</t>
-  </si>
-  <si>
-    <t>          2)  Ball roling on fingers and body is a foul. Carry is also foul.</t>
-  </si>
-  <si>
-    <t>          3) 1 body pass is allowed.</t>
-  </si>
-  <si>
-    <t>Only the captain can dispute/talk about any issue with the refree/organizer</t>
-  </si>
-  <si>
-    <t>Game will continue until referee calls off, should not ask for re service.</t>
-  </si>
-  <si>
-    <t>Winners and Runners will be presented with trophies.</t>
-  </si>
-  <si>
-    <t>Snacks, Tea and Water will be served.</t>
-  </si>
-  <si>
-    <t>*** Team Numbers will be decided on the day of the tournament itself by a draw between captains ****</t>
-  </si>
-  <si>
-    <t>All Players must be in ground by 1:30 PM</t>
-  </si>
-  <si>
-    <t>Game Format: 7 Team Round Robin</t>
-  </si>
-  <si>
-    <t>Points: 21 point 1 Set Game will be played (Court swap after first 10 points i.e. which ever team reaches to 10 points, courts shall be changed)</t>
-  </si>
-  <si>
-    <t>           Teams will reset to their desired Original Position after court swap after 10 points.</t>
-  </si>
-  <si>
-    <t>           Each team will get a chance to play against every other team (6 game gurantee)</t>
-  </si>
-  <si>
     <t>Ismail</t>
   </si>
   <si>
@@ -273,15 +221,6 @@
     <t>Ranjith</t>
   </si>
   <si>
-    <t>If a player touches the line during Service, It will be a straight point to opposite team no warnings will be issued.</t>
-  </si>
-  <si>
-    <t>           Semis and Finals will be a game with best of 3 sets. (Each Set - 15 points) accordance with original VB Standards.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  If we  are running short of time , then we will go for 30 points game for semis with one swap at 15 points.</t>
-  </si>
-  <si>
     <t>Chronos (Peddi)</t>
   </si>
   <si>
@@ -304,18 +243,6 @@
   </si>
   <si>
     <t>Decoders (Ajith)</t>
-  </si>
-  <si>
-    <t>Referee decision will be final. If refree is unsure of what to call on a certain scenario, he can take help (Naren/Sridhar/Praveen)</t>
-  </si>
-  <si>
-    <t>Back row player attacking a ball inside the front zone (the area inside the 3M/10-foot line) when at the moment of contact, the ball is completely above the net is illegal.</t>
-  </si>
-  <si>
-    <t>If palyer is not available or not on time .. They need to continue with their rest of the players.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> i.e Back row player cannot jump across the line (front zone) to spike</t>
   </si>
   <si>
     <t>VB 2.0 – Rules</t>
@@ -394,7 +321,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,12 +433,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -681,24 +602,24 @@
   </borders>
   <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -734,9 +655,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -744,8 +662,34 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -756,15 +700,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -789,9 +724,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="18" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -804,23 +736,6 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1160,35 +1075,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="29" customHeight="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:15" ht="21">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="F2" s="39" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="F2" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="J2" s="32" t="s">
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="J2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="33"/>
+      <c r="K2" s="39"/>
       <c r="M2" s="13"/>
     </row>
     <row r="3" spans="1:15" ht="20">
@@ -1216,26 +1131,26 @@
       <c r="L3" s="5"/>
       <c r="M3" s="15"/>
       <c r="N3" s="16" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="O3" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="16">
-      <c r="A4" s="38">
+      <c r="A4" s="32">
         <v>0.58333333333333337</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="34">
+        <v>73</v>
+      </c>
+      <c r="F4" s="40">
         <v>0.77777777777777779</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -1245,7 +1160,7 @@
         <v>7</v>
       </c>
       <c r="I4" s="10"/>
-      <c r="J4" s="36">
+      <c r="J4" s="42">
         <v>0.8125</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -1256,24 +1171,24 @@
         <v>15</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="O4" s="22" t="s">
-        <v>92</v>
+        <v>27</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="16">
-      <c r="A5" s="38"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="9" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F5" s="35"/>
+        <v>68</v>
+      </c>
+      <c r="F5" s="41"/>
       <c r="G5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1281,7 +1196,7 @@
         <v>8</v>
       </c>
       <c r="I5" s="10"/>
-      <c r="J5" s="36"/>
+      <c r="J5" s="42"/>
       <c r="K5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1289,303 +1204,317 @@
         <v>16</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="O5" s="22" t="s">
-        <v>86</v>
+        <v>50</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
+      <c r="B6" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="46"/>
+      <c r="D6" s="47"/>
       <c r="M6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="O6" s="22" t="s">
-        <v>87</v>
+        <v>44</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15">
-      <c r="A7" s="38">
+      <c r="A7" s="32">
         <v>0.61111111111111105</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="M7" s="15" t="s">
         <v>18</v>
       </c>
       <c r="N7" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="O7" s="22" t="s">
-        <v>93</v>
+        <v>42</v>
+      </c>
+      <c r="O7" s="21" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15">
-      <c r="A8" s="38"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="9" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="M8" s="15" t="s">
         <v>19</v>
       </c>
       <c r="N8" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="O8" s="22" t="s">
-        <v>88</v>
+        <v>31</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
+      <c r="B9" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="46"/>
+      <c r="D9" s="47"/>
       <c r="M9" s="14" t="s">
         <v>20</v>
       </c>
       <c r="N9" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="O9" s="22" t="s">
-        <v>89</v>
+        <v>46</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15">
-      <c r="A10" s="38">
+      <c r="A10" s="32">
         <v>0.63888888888888895</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="M10" s="15" t="s">
         <v>21</v>
       </c>
       <c r="N10" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="O10" s="22" t="s">
-        <v>90</v>
+        <v>40</v>
+      </c>
+      <c r="O10" s="21" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15">
-      <c r="A11" s="38"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="9" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15">
       <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
+      <c r="B12" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
       <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:15" ht="15">
-      <c r="A13" s="38">
+      <c r="A13" s="32">
         <v>0.66666666666666663</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15">
-      <c r="A14" s="38"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="9" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15">
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
+      <c r="B15" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="26"/>
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:15" ht="15">
-      <c r="A16" s="38">
+      <c r="A16" s="32">
         <v>0.69444444444444453</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15">
-      <c r="A17" s="38"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="9" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="26"/>
+      <c r="B18" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="34"/>
+      <c r="D18" s="35"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="46">
+      <c r="A19" s="30">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="46"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
     </row>
     <row r="21" spans="1:4" ht="15">
-      <c r="A21" s="38">
+      <c r="A21" s="32">
         <v>0.72222222222222221</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>87</v>
+        <v>70</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>67</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15">
-      <c r="A22" s="38"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>92</v>
+        <v>69</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>72</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15">
       <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="29"/>
+      <c r="B23" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="25"/>
+      <c r="D23" s="26"/>
     </row>
     <row r="24" spans="1:4" ht="15">
-      <c r="A24" s="38">
+      <c r="A24" s="32">
         <v>0.75</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15">
-      <c r="A25" s="38"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="9" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="45"/>
+      <c r="B26" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="28"/>
+      <c r="D26" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F2:H2"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="A19:A20"/>
@@ -1594,20 +1523,6 @@
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B23:D23"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -1639,164 +1554,164 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18">
+      <c r="A3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18">
+      <c r="A4" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="E4" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="G4" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="19" t="s">
+    </row>
+    <row r="5" spans="1:7" ht="18">
+      <c r="A5" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="B5" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="18">
-      <c r="A3" s="20" t="s">
+      <c r="D5" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="F5" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="G5" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="19" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="18">
+      <c r="A6" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="18">
-      <c r="A4" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="F6" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="G6" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="20" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="18">
+      <c r="A7" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="C7" s="18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="18">
-      <c r="A5" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="E7" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="F7" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="G7" s="18" t="s">
         <v>65</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="18">
-      <c r="A6" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="18">
-      <c r="A7" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1811,154 +1726,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="16">
-      <c r="A1" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="16">
-      <c r="A2" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="16">
-      <c r="A3" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="16">
-      <c r="A4" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="16">
-      <c r="A5" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="16">
-      <c r="A6" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="16">
-      <c r="A7" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="16">
-      <c r="A9" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="16">
-      <c r="A10" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="16">
-      <c r="A11" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="16">
-      <c r="A13" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="16">
-      <c r="A14" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="16">
-      <c r="A15" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="16">
-      <c r="A16" s="17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="16">
-      <c r="A17" s="17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="16">
-      <c r="A18" s="17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="16">
-      <c r="A19" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="16">
-      <c r="A20" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="16">
-      <c r="A21" s="17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="16">
-      <c r="A22" s="17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="16">
-      <c r="A23" s="23" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="16">
-      <c r="A24" s="17"/>
-    </row>
-    <row r="25" spans="1:1" ht="16">
-      <c r="A25" s="17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="16">
-      <c r="A26" s="17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="16">
-      <c r="A28" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1968,123 +1739,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="16">
-      <c r="A1" s="49" t="s">
-        <v>98</v>
+      <c r="A1" s="23" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="16">
-      <c r="A2" s="48" t="s">
-        <v>99</v>
+      <c r="A2" s="22" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="16">
-      <c r="A3" s="48" t="s">
-        <v>100</v>
+      <c r="A3" s="22" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="16">
-      <c r="A4" s="48" t="s">
-        <v>101</v>
+      <c r="A4" s="22" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="16">
-      <c r="A5" s="48" t="s">
-        <v>102</v>
+      <c r="A5" s="22" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="16">
-      <c r="A6" s="48" t="s">
-        <v>103</v>
+      <c r="A6" s="22" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="16">
-      <c r="A7" s="48" t="s">
-        <v>104</v>
+      <c r="A7" s="22" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="16">
-      <c r="A8" s="48" t="s">
-        <v>105</v>
+      <c r="A8" s="22" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="16">
-      <c r="A9" s="48" t="s">
-        <v>106</v>
+      <c r="A9" s="22" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="16">
-      <c r="A10" s="48" t="s">
-        <v>107</v>
+      <c r="A10" s="22" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="16">
-      <c r="A11" s="48" t="s">
-        <v>108</v>
+      <c r="A11" s="22" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="16">
-      <c r="A12" s="48" t="s">
-        <v>109</v>
+      <c r="A12" s="22" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="16">
-      <c r="A13" s="48" t="s">
-        <v>110</v>
+      <c r="A13" s="22" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="16">
-      <c r="A14" s="48" t="s">
-        <v>111</v>
+      <c r="A14" s="22" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="16">
-      <c r="A15" s="48" t="s">
-        <v>112</v>
+      <c r="A15" s="22" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="16">
-      <c r="A16" s="48" t="s">
-        <v>113</v>
+      <c r="A16" s="22" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="16">
-      <c r="A17" s="48" t="s">
-        <v>114</v>
+      <c r="A17" s="22" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="16">
-      <c r="A18" s="48" t="s">
-        <v>115</v>
+      <c r="A18" s="22" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="16">
-      <c r="A19" s="48" t="s">
-        <v>116</v>
+      <c r="A19" s="22" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="16">
-      <c r="A20" s="48" t="s">
-        <v>117</v>
+      <c r="A20" s="22" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="16">
-      <c r="A21" s="48" t="s">
-        <v>118</v>
+      <c r="A21" s="22" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="16">
-      <c r="A22" s="48" t="s">
-        <v>119</v>
+      <c r="A22" s="22" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="16">
-      <c r="A23" s="48" t="s">
-        <v>120</v>
+      <c r="A23" s="22" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="16">
-      <c r="A24" s="48" t="s">
-        <v>121</v>
+      <c r="A24" s="22" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>